<commit_message>
feat: fix database module
</commit_message>
<xml_diff>
--- a/backend/uploads/Database.xlsx
+++ b/backend/uploads/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghks2\Bems\4msys\Database_poll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guccin/Code/Bems/bems_vue/backend/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A6B2C3-E1E5-4EDB-B57D-F77351A6E4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A51281A-DE14-2746-A828-ED9672FB7CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -442,9 +442,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>데이터를</t>
@@ -453,19 +453,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>꺼낼</t>
@@ -474,19 +474,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>데이터베이스의</t>
@@ -495,7 +495,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -509,7 +509,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -520,9 +520,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>데이터를</t>
@@ -531,19 +531,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>쓸</t>
@@ -552,7 +552,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -562,9 +562,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>데이터베이스</t>
@@ -573,7 +573,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -587,7 +587,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -597,9 +597,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>은</t>
@@ -608,7 +608,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -618,9 +618,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>에서</t>
@@ -629,7 +629,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -639,9 +639,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>로</t>
@@ -650,19 +650,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>어떤</t>
@@ -671,19 +671,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>행동을</t>
@@ -692,19 +692,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>할지</t>
@@ -713,19 +713,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>선택한다</t>
@@ -734,20 +734,40 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>. 
-Insert: log</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>i</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nsert: log</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>값</t>
@@ -756,188 +776,30 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">삽입
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Update: log</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>값</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>갱신</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>나머지</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>데이터는</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>서로</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>존재할때만</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>갱신</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>삽입</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t xml:space="preserve">
@@ -947,19 +809,208 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Insert_ecosian: ecosian</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>u</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>pdate: log</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>값</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>갱신</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>나머지</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>데이터는</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>서로</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>존재할때만</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>갱신</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>i</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nsert_ecosian: ecosian</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>형태로</t>
@@ -968,19 +1019,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>데이터를</t>
@@ -989,19 +1040,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>삽입하나</t>
@@ -1010,20 +1061,40 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>.
-Update_ecosian: ecosian</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>u</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>pdate_ecosian: ecosian</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>형태로</t>
@@ -1032,7 +1103,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1042,9 +1113,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>만</t>
@@ -1053,19 +1124,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>데이터</t>
@@ -1074,19 +1145,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>가져오고</t>
@@ -1095,7 +1166,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1105,9 +1176,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>으로</t>
@@ -1116,19 +1187,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>처리</t>
@@ -1137,7 +1208,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1151,9 +1222,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>에코시안</t>
@@ -1162,7 +1233,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1172,9 +1243,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>사용시</t>
@@ -1183,20 +1254,30 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-M_Site_Cd</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>M_Site_Cd</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>가</t>
@@ -1205,19 +1286,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>필요한</t>
@@ -1226,19 +1307,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>경우</t>
@@ -1247,19 +1328,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>사용한다</t>
@@ -1268,7 +1349,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1279,9 +1360,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>즉</t>
@@ -1290,7 +1371,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1300,9 +1381,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>에코시안으로</t>
@@ -1311,7 +1392,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1321,9 +1402,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>하는</t>
@@ -1332,19 +1413,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>경우</t>
@@ -1353,7 +1434,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1363,9 +1444,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>을</t>
@@ -1374,19 +1455,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>표시하고</t>
@@ -1395,19 +1476,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>일반적인</t>
@@ -1416,7 +1497,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1426,9 +1507,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>인</t>
@@ -1437,19 +1518,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>경우</t>
@@ -1458,19 +1539,19 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
             <charset val="129"/>
           </rPr>
           <t>비워준다</t>
@@ -1479,7 +1560,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1648,7 +1729,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>DB_Id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1763,10 +1844,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4msys</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>realtime_table</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1827,10 +1904,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>121.140.99.242</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>pms</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1880,6 +1953,18 @@
   </si>
   <si>
     <t>ctrlvalue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>121.140.99.242.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4msys!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1887,7 +1972,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1935,6 +2020,21 @@
       <color indexed="81"/>
       <name val="돋움"/>
       <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="2"/>
       <charset val="129"/>
     </font>
   </fonts>
@@ -2359,43 +2459,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="5.5" style="6" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.25" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.08203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.08203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11" style="6" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.25" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.58203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="6" customWidth="1"/>
     <col min="9" max="9" width="16.83203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="16.58203125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="10" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" style="10" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" style="5" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="15.08203125" style="8" customWidth="1"/>
+    <col min="14" max="14" width="15" style="8" customWidth="1"/>
     <col min="15" max="15" width="14.83203125" style="8" customWidth="1"/>
     <col min="16" max="16" width="13.83203125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="16.25" style="9" customWidth="1"/>
-    <col min="18" max="18" width="8.25" style="7" customWidth="1"/>
-    <col min="19" max="19" width="9.25" style="7" customWidth="1"/>
-    <col min="20" max="21" width="8.58203125" style="7"/>
+    <col min="17" max="17" width="16.1640625" style="9" customWidth="1"/>
+    <col min="18" max="18" width="8.1640625" style="7" customWidth="1"/>
+    <col min="19" max="19" width="9.1640625" style="7" customWidth="1"/>
+    <col min="20" max="21" width="8.5" style="7"/>
     <col min="22" max="22" width="14.33203125" style="7" customWidth="1"/>
     <col min="23" max="23" width="17.83203125" style="7" customWidth="1"/>
     <col min="24" max="24" width="16" style="7" customWidth="1"/>
     <col min="25" max="25" width="17.83203125" style="7" customWidth="1"/>
     <col min="26" max="26" width="16" style="7" customWidth="1"/>
-    <col min="27" max="16384" width="8.58203125" style="6"/>
+    <col min="27" max="16384" width="8.5" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2448,7 +2548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2468,16 +2568,16 @@
         <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>6</v>
@@ -2489,116 +2589,179 @@
         <v>5</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>22</v>
       </c>
       <c r="P2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3306</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5432</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="6">
+      <c r="H5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="6">
         <v>5432</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E6" s="6">
         <v>3</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="G6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>51</v>
+      <c r="Q6" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="6">
-        <v>5432</v>
-      </c>
-      <c r="E4" s="6">
-        <v>3</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>35</v>
+    <row r="7" spans="1:17">
+      <c r="A7" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2611,24 +2774,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="16.25" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2639,10 +2802,10 @@
         <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>29</v>
@@ -2651,7 +2814,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -2662,19 +2825,19 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>1001030001</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2685,19 +2848,19 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>1001030002</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2708,19 +2871,19 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4">
         <v>1001030003</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2731,19 +2894,19 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5">
         <v>1001030004</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="16.5" customHeight="1">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2754,19 +2917,19 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6">
         <v>1001030005</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2777,19 +2940,19 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7">
         <v>1001030006</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2800,19 +2963,19 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8">
         <v>1001030007</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2823,7 +2986,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2832,6 +2995,11 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: xml parser 추가
</commit_message>
<xml_diff>
--- a/backend/uploads/Database.xlsx
+++ b/backend/uploads/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guccin/Code/Bems/bems_vue/backend/uploads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghks2.DESKTOP-DH3JS7E\4msys\bems_vue\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A51281A-DE14-2746-A828-ED9672FB7CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B911102-E7EB-4E13-88DD-AA0E956C5EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -1729,7 +1729,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>DB_Id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1966,13 +1966,17 @@
   <si>
     <t>4msys!</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2111,7 +2115,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2121,9 +2125,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2131,9 +2132,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2459,308 +2457,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="16.5" style="10" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="5" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="5" customWidth="1"/>
-    <col min="14" max="14" width="15" style="8" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" style="8" customWidth="1"/>
-    <col min="16" max="16" width="13.83203125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="16.1640625" style="9" customWidth="1"/>
-    <col min="18" max="18" width="8.1640625" style="7" customWidth="1"/>
-    <col min="19" max="19" width="9.1640625" style="7" customWidth="1"/>
-    <col min="20" max="21" width="8.5" style="7"/>
-    <col min="22" max="22" width="14.33203125" style="7" customWidth="1"/>
-    <col min="23" max="23" width="17.83203125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="16" style="7" customWidth="1"/>
-    <col min="25" max="25" width="17.83203125" style="7" customWidth="1"/>
-    <col min="26" max="26" width="16" style="7" customWidth="1"/>
-    <col min="27" max="16384" width="8.5" style="6"/>
+    <col min="1" max="1" width="5.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="23.796875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.296875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="5" customWidth="1"/>
+    <col min="9" max="9" width="16.796875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="8" customWidth="1"/>
+    <col min="11" max="11" width="14.296875" style="8" customWidth="1"/>
+    <col min="12" max="12" width="14.296875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13.296875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="15" style="6" customWidth="1"/>
+    <col min="15" max="15" width="14.796875" style="6" customWidth="1"/>
+    <col min="16" max="16" width="13.796875" style="7" customWidth="1"/>
+    <col min="17" max="17" width="16.19921875" style="7" customWidth="1"/>
+    <col min="18" max="18" width="8.19921875" style="5" customWidth="1"/>
+    <col min="19" max="19" width="9.19921875" style="5" customWidth="1"/>
+    <col min="20" max="21" width="8.5" style="5"/>
+    <col min="22" max="22" width="14.296875" style="5" customWidth="1"/>
+    <col min="23" max="23" width="17.796875" style="5" customWidth="1"/>
+    <col min="24" max="24" width="16" style="5" customWidth="1"/>
+    <col min="25" max="25" width="17.796875" style="5" customWidth="1"/>
+    <col min="26" max="26" width="16" style="5" customWidth="1"/>
+    <col min="27" max="16384" width="8.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="6">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>3306</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3306</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q3" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="6">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
-        <v>3306</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5432</v>
+      </c>
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="5" t="s">
+      <c r="F5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="5">
+        <v>5432</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="O3" s="8" t="s">
+      <c r="L6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="9" t="s">
+      <c r="N6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="6">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="6">
-        <v>5432</v>
-      </c>
-      <c r="E5" s="6">
-        <v>3</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="6">
-        <v>5432</v>
-      </c>
-      <c r="E6" s="6">
-        <v>3</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2777,21 +2775,21 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.796875" customWidth="1"/>
+    <col min="2" max="2" width="12.296875" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.19921875" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2804,7 +2802,7 @@
       <c r="D1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2814,8 +2812,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
@@ -2837,7 +2835,7 @@
         <v>1001030001</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2860,7 +2858,7 @@
         <v>1001030002</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2883,7 +2881,7 @@
         <v>1001030003</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2906,7 +2904,7 @@
         <v>1001030004</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" customHeight="1">
+    <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2929,7 +2927,7 @@
         <v>1001030005</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2952,7 +2950,7 @@
         <v>1001030006</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2975,7 +2973,7 @@
         <v>1001030007</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2998,7 +2996,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>59</v>
       </c>

</xml_diff>